<commit_message>
screenshoot functionality add in testng listener class
</commit_message>
<xml_diff>
--- a/src/test/resources/QaFoxTestData.xlsx
+++ b/src/test/resources/QaFoxTestData.xlsx
@@ -5,42 +5,94 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5466b3f5faf63203/Software Testing/Manual testing/Qafox(OpenCart) project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naimn\DEV\IDE\eclipse\tutorialNinja\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EF6792A3-7C49-432E-80FC-D8374A42BB8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB7B40B-C16F-4F20-98BD-725AB2C9A5C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="13665" xr2:uid="{ED0386A5-799D-4F0B-8E60-1F40B7F4AF16}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="18900" windowHeight="10245" xr2:uid="{ED0386A5-799D-4F0B-8E60-1F40B7F4AF16}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Customer Registration Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+  <si>
+    <t>pence</t>
+  </si>
+  <si>
+    <t>teyf6464646</t>
+  </si>
+  <si>
+    <t>mike 2</t>
+  </si>
+  <si>
+    <t>mike 3</t>
+  </si>
+  <si>
+    <t>mike 4</t>
+  </si>
+  <si>
+    <t>first name</t>
+  </si>
+  <si>
+    <t>last name</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>telephone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mike 1 </t>
+  </si>
+  <si>
+    <t>mike1@gmail.com</t>
+  </si>
+  <si>
+    <t>mike2@gmail.com</t>
+  </si>
+  <si>
+    <t>mike3@gmail.com</t>
+  </si>
+  <si>
+    <t>mike4@gmail.com</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -54,7 +106,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -62,14 +114,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -382,9 +449,131 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45177BA7-62E4-40E2-83F1-DE3E6C81C00F}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+    <col min="4" max="4" width="29.28515625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="3">
+        <v>7474847575</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="3">
+        <v>7474847575</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3">
+        <v>7474847575</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="3">
+        <v>7474847575</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D75B51D-8CC4-4630-A258-989507A3DD70}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69F809BD-6DDF-46FD-A3E4-009F696FD236}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>